<commit_message>
Updating sheet with ROC analysis
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="339">
   <si>
     <t>Accuracy</t>
   </si>
@@ -821,16 +821,348 @@
   <si>
     <t>1 7
 20 382</t>
+  </si>
+  <si>
+    <t>Análisis ROC</t>
+  </si>
+  <si>
+    <t>SVM 5-fold Cross Validation + GridSearch 2-fold 5 times</t>
+  </si>
+  <si>
+    <t>SVM kernel='linear', class_weight='balanced'</t>
+  </si>
+  <si>
+    <t>AUC</t>
+  </si>
+  <si>
+    <t>Best threshold</t>
+  </si>
+  <si>
+    <t>0.741</t>
+  </si>
+  <si>
+    <t>0.591447</t>
+  </si>
+  <si>
+    <t>0.719</t>
+  </si>
+  <si>
+    <t>0.534865</t>
+  </si>
+  <si>
+    <t>0.514</t>
+  </si>
+  <si>
+    <t>0.225341</t>
+  </si>
+  <si>
+    <t>0.585</t>
+  </si>
+  <si>
+    <t>0.265185</t>
+  </si>
+  <si>
+    <t>0.752</t>
+  </si>
+  <si>
+    <t>0.129189</t>
+  </si>
+  <si>
+    <t>0.716</t>
+  </si>
+  <si>
+    <t>0.102358</t>
+  </si>
+  <si>
+    <t>0.575</t>
+  </si>
+  <si>
+    <t>0.094650</t>
+  </si>
+  <si>
+    <t>0.656</t>
+  </si>
+  <si>
+    <t>0.088114</t>
+  </si>
+  <si>
+    <t>0.600</t>
+  </si>
+  <si>
+    <t>0.070869</t>
+  </si>
+  <si>
+    <t>0.460</t>
+  </si>
+  <si>
+    <t>0.076602</t>
+  </si>
+  <si>
+    <t>0.540</t>
+  </si>
+  <si>
+    <t>0.926604</t>
+  </si>
+  <si>
+    <t>0.766</t>
+  </si>
+  <si>
+    <t>0.060680</t>
+  </si>
+  <si>
+    <t>0.757</t>
+  </si>
+  <si>
+    <t>0.067359</t>
+  </si>
+  <si>
+    <t>0.605</t>
+  </si>
+  <si>
+    <t>0.061953</t>
+  </si>
+  <si>
+    <t>0.610</t>
+  </si>
+  <si>
+    <t>0.080192</t>
+  </si>
+  <si>
+    <t>0.548</t>
+  </si>
+  <si>
+    <t>0.044148</t>
+  </si>
+  <si>
+    <t>0.718</t>
+  </si>
+  <si>
+    <t>0.043037</t>
+  </si>
+  <si>
+    <t>0.486</t>
+  </si>
+  <si>
+    <t>0.028681</t>
+  </si>
+  <si>
+    <t>0.454</t>
+  </si>
+  <si>
+    <t>0.668</t>
+  </si>
+  <si>
+    <t>0.041987</t>
+  </si>
+  <si>
+    <t>0.638</t>
+  </si>
+  <si>
+    <t>0.025183</t>
+  </si>
+  <si>
+    <t>0.513</t>
+  </si>
+  <si>
+    <t>0.017158</t>
+  </si>
+  <si>
+    <t>0.620</t>
+  </si>
+  <si>
+    <t>0.017591</t>
+  </si>
+  <si>
+    <t>Best threshold calculado como el punto cuya distancia a la esquina superior izquierda (+TPR -FPR) es menor</t>
+  </si>
+  <si>
+    <t>Resultados con nuevo threshold</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>Matriz de confusion</t>
+  </si>
+  <si>
+    <t>0.6878048780487804</t>
+  </si>
+  <si>
+    <t>151 74
+54 131</t>
+  </si>
+  <si>
+    <t>0.7393162393162392</t>
+  </si>
+  <si>
+    <t>173 52
+70 115</t>
+  </si>
+  <si>
+    <t>F1 inversa</t>
+  </si>
+  <si>
+    <t>0.5195121951219512</t>
+  </si>
+  <si>
+    <t>54 50
+147 159</t>
+  </si>
+  <si>
+    <t>0.39230769230769236</t>
+  </si>
+  <si>
+    <t>51 53
+105 201</t>
+  </si>
+  <si>
+    <t>Aquí hay más accuracy que a la izquierda</t>
+  </si>
+  <si>
+    <t>0.7317073170731707</t>
+  </si>
+  <si>
+    <t>37 16
+94 263</t>
+  </si>
+  <si>
+    <t>0.36363636363636365</t>
+  </si>
+  <si>
+    <t>42 11
+136 221</t>
+  </si>
+  <si>
+    <t>0.6682926829268293</t>
+  </si>
+  <si>
+    <t>17 20
+116 257</t>
+  </si>
+  <si>
+    <t>0.23148148148148145</t>
+  </si>
+  <si>
+    <t>25 12
+154 219</t>
+  </si>
+  <si>
+    <t>0.7195121951219512</t>
+  </si>
+  <si>
+    <t>14 14
+101 281</t>
+  </si>
+  <si>
+    <t>0.10256410256410256</t>
+  </si>
+  <si>
+    <t>12 16
+194 188</t>
+  </si>
+  <si>
+    <t>0.7609756097560976</t>
+  </si>
+  <si>
+    <t>17 9
+89 295</t>
+  </si>
+  <si>
+    <t>0.26277372262773724</t>
+  </si>
+  <si>
+    <t>18 8
+93 291</t>
+  </si>
+  <si>
+    <t>0.7560975609756098</t>
+  </si>
+  <si>
+    <t>12 13
+87 298</t>
+  </si>
+  <si>
+    <t>0.2682926829268293</t>
+  </si>
+  <si>
+    <t>11 14
+46 339</t>
+  </si>
+  <si>
+    <t>0.5121951219512195</t>
+  </si>
+  <si>
+    <t>12 6
+194 198</t>
+  </si>
+  <si>
+    <t>0.20512820512820512</t>
+  </si>
+  <si>
+    <t>12 6
+87 305</t>
+  </si>
+  <si>
+    <t>0.4878048780487805</t>
+  </si>
+  <si>
+    <t>7 5
+205 193</t>
+  </si>
+  <si>
+    <t>0.056338028169014086</t>
+  </si>
+  <si>
+    <t>6 6
+195 203</t>
+  </si>
+  <si>
+    <t>0.8975609756097561</t>
+  </si>
+  <si>
+    <t>4 6
+36 364</t>
+  </si>
+  <si>
+    <t>0.07194244604316548</t>
+  </si>
+  <si>
+    <t>5 5
+124 276</t>
+  </si>
+  <si>
+    <t>0.40487804878048783</t>
+  </si>
+  <si>
+    <t>4 4
+240 162</t>
+  </si>
+  <si>
+    <t>0.05405405405405406</t>
+  </si>
+  <si>
+    <t>5 3
+172 230</t>
+  </si>
+  <si>
+    <t>e</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1035,7 +1367,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1092,6 +1424,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1406,10 +1745,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N79"/>
+  <dimension ref="A1:N118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="75" workbookViewId="0">
-      <selection activeCell="J51" sqref="J51"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="75" workbookViewId="0">
+      <selection activeCell="G87" sqref="G87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3059,6 +3398,658 @@
       <c r="F79" s="32"/>
       <c r="G79" s="32"/>
     </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A82" s="44" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A84" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B84" s="48" t="s">
+        <v>240</v>
+      </c>
+      <c r="C84" s="12"/>
+      <c r="H84" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="I84" s="48" t="s">
+        <v>240</v>
+      </c>
+      <c r="J84" s="12"/>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A85" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="B85" s="41" t="s">
+        <v>241</v>
+      </c>
+      <c r="C85" s="34" t="s">
+        <v>242</v>
+      </c>
+      <c r="H85" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="I85" s="41" t="s">
+        <v>241</v>
+      </c>
+      <c r="J85" s="34" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A86" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="B86" s="37" t="s">
+        <v>243</v>
+      </c>
+      <c r="C86" s="35" t="s">
+        <v>244</v>
+      </c>
+      <c r="H86" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="I86" s="37" t="s">
+        <v>245</v>
+      </c>
+      <c r="J86" s="35" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A87" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="B87" s="37" t="s">
+        <v>247</v>
+      </c>
+      <c r="C87" s="35" t="s">
+        <v>248</v>
+      </c>
+      <c r="G87" t="s">
+        <v>338</v>
+      </c>
+      <c r="H87" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="I87" s="37" t="s">
+        <v>249</v>
+      </c>
+      <c r="J87" s="35" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A88" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="B88" s="37" t="s">
+        <v>251</v>
+      </c>
+      <c r="C88" s="35" t="s">
+        <v>252</v>
+      </c>
+      <c r="H88" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="I88" s="37" t="s">
+        <v>253</v>
+      </c>
+      <c r="J88" s="35" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A89" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="B89" s="37" t="s">
+        <v>255</v>
+      </c>
+      <c r="C89" s="35" t="s">
+        <v>256</v>
+      </c>
+      <c r="H89" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="I89" s="37" t="s">
+        <v>257</v>
+      </c>
+      <c r="J89" s="35" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A90" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="B90" s="37" t="s">
+        <v>259</v>
+      </c>
+      <c r="C90" s="35" t="s">
+        <v>260</v>
+      </c>
+      <c r="H90" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="I90" s="50" t="s">
+        <v>261</v>
+      </c>
+      <c r="J90" s="51" t="s">
+        <v>262</v>
+      </c>
+      <c r="K90" t="s">
+        <v>263</v>
+      </c>
+      <c r="L90" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A91" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="B91" s="37" t="s">
+        <v>265</v>
+      </c>
+      <c r="C91" s="35" t="s">
+        <v>266</v>
+      </c>
+      <c r="H91" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="I91" s="37" t="s">
+        <v>267</v>
+      </c>
+      <c r="J91" s="35" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A92" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="B92" s="37" t="s">
+        <v>269</v>
+      </c>
+      <c r="C92" s="35" t="s">
+        <v>270</v>
+      </c>
+      <c r="H92" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="I92" s="37" t="s">
+        <v>271</v>
+      </c>
+      <c r="J92" s="35" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A93" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="B93" s="37" t="s">
+        <v>273</v>
+      </c>
+      <c r="C93" s="35" t="s">
+        <v>274</v>
+      </c>
+      <c r="H93" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="I93" s="37" t="s">
+        <v>275</v>
+      </c>
+      <c r="J93" s="35" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A94" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="B94" s="50" t="s">
+        <v>277</v>
+      </c>
+      <c r="C94" s="51" t="s">
+        <v>278</v>
+      </c>
+      <c r="H94" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="I94" s="50" t="s">
+        <v>279</v>
+      </c>
+      <c r="J94" s="51" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A95" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="B95" s="37" t="s">
+        <v>280</v>
+      </c>
+      <c r="C95" s="35" t="s">
+        <v>281</v>
+      </c>
+      <c r="H95" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="I95" s="37" t="s">
+        <v>282</v>
+      </c>
+      <c r="J95" s="35" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A96" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="B96" s="37" t="s">
+        <v>284</v>
+      </c>
+      <c r="C96" s="35" t="s">
+        <v>285</v>
+      </c>
+      <c r="H96" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="I96" s="37" t="s">
+        <v>286</v>
+      </c>
+      <c r="J96" s="35" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A97" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="B97" s="38"/>
+      <c r="C97" s="33"/>
+      <c r="H97" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="I97" s="38"/>
+      <c r="J97" s="33"/>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A99" s="52" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A105" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B105" s="48" t="s">
+        <v>240</v>
+      </c>
+      <c r="C105" s="12"/>
+      <c r="D105" s="13"/>
+      <c r="H105" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="I105" s="48" t="s">
+        <v>240</v>
+      </c>
+      <c r="J105" s="12"/>
+      <c r="K105" s="13"/>
+    </row>
+    <row r="106" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A106" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="B106" s="41" t="s">
+        <v>290</v>
+      </c>
+      <c r="C106" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="D106" s="53" t="s">
+        <v>291</v>
+      </c>
+      <c r="H106" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="I106" s="41" t="s">
+        <v>290</v>
+      </c>
+      <c r="J106" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="K106" s="53" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="A107" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="B107" s="35" t="s">
+        <v>244</v>
+      </c>
+      <c r="C107" s="35" t="s">
+        <v>292</v>
+      </c>
+      <c r="D107" s="54" t="s">
+        <v>293</v>
+      </c>
+      <c r="H107" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="I107" s="35" t="s">
+        <v>246</v>
+      </c>
+      <c r="J107" s="35" t="s">
+        <v>294</v>
+      </c>
+      <c r="K107" s="54" t="s">
+        <v>295</v>
+      </c>
+      <c r="L107" s="52" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="108" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="A108" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="B108" s="35" t="s">
+        <v>248</v>
+      </c>
+      <c r="C108" s="35" t="s">
+        <v>297</v>
+      </c>
+      <c r="D108" s="54" t="s">
+        <v>298</v>
+      </c>
+      <c r="H108" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="I108" s="35" t="s">
+        <v>250</v>
+      </c>
+      <c r="J108" s="35" t="s">
+        <v>299</v>
+      </c>
+      <c r="K108" s="54" t="s">
+        <v>300</v>
+      </c>
+      <c r="L108" s="52" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="A109" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="B109" s="35" t="s">
+        <v>252</v>
+      </c>
+      <c r="C109" s="35" t="s">
+        <v>302</v>
+      </c>
+      <c r="D109" s="54" t="s">
+        <v>303</v>
+      </c>
+      <c r="H109" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="I109" s="35" t="s">
+        <v>254</v>
+      </c>
+      <c r="J109" s="35" t="s">
+        <v>304</v>
+      </c>
+      <c r="K109" s="54" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="110" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="A110" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="B110" s="35" t="s">
+        <v>256</v>
+      </c>
+      <c r="C110" s="35" t="s">
+        <v>306</v>
+      </c>
+      <c r="D110" s="54" t="s">
+        <v>307</v>
+      </c>
+      <c r="H110" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="I110" s="35" t="s">
+        <v>258</v>
+      </c>
+      <c r="J110" s="35" t="s">
+        <v>308</v>
+      </c>
+      <c r="K110" s="54" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="111" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="A111" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="B111" s="35" t="s">
+        <v>260</v>
+      </c>
+      <c r="C111" s="35" t="s">
+        <v>310</v>
+      </c>
+      <c r="D111" s="54" t="s">
+        <v>311</v>
+      </c>
+      <c r="H111" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="I111" s="51" t="s">
+        <v>262</v>
+      </c>
+      <c r="J111" s="35" t="s">
+        <v>312</v>
+      </c>
+      <c r="K111" s="54" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="A112" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="B112" s="35" t="s">
+        <v>266</v>
+      </c>
+      <c r="C112" s="35" t="s">
+        <v>314</v>
+      </c>
+      <c r="D112" s="54" t="s">
+        <v>315</v>
+      </c>
+      <c r="H112" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="I112" s="35" t="s">
+        <v>268</v>
+      </c>
+      <c r="J112" s="35" t="s">
+        <v>316</v>
+      </c>
+      <c r="K112" s="54" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="A113" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="B113" s="35" t="s">
+        <v>270</v>
+      </c>
+      <c r="C113" s="35" t="s">
+        <v>318</v>
+      </c>
+      <c r="D113" s="54" t="s">
+        <v>319</v>
+      </c>
+      <c r="H113" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="I113" s="35" t="s">
+        <v>272</v>
+      </c>
+      <c r="J113" s="35" t="s">
+        <v>320</v>
+      </c>
+      <c r="K113" s="54" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="A114" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="B114" s="35" t="s">
+        <v>274</v>
+      </c>
+      <c r="C114" s="35" t="s">
+        <v>322</v>
+      </c>
+      <c r="D114" s="54" t="s">
+        <v>323</v>
+      </c>
+      <c r="H114" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="I114" s="35" t="s">
+        <v>276</v>
+      </c>
+      <c r="J114" s="35" t="s">
+        <v>324</v>
+      </c>
+      <c r="K114" s="54" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="A115" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="B115" s="51" t="s">
+        <v>278</v>
+      </c>
+      <c r="C115" s="35" t="s">
+        <v>326</v>
+      </c>
+      <c r="D115" s="54" t="s">
+        <v>327</v>
+      </c>
+      <c r="H115" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="I115" s="51" t="s">
+        <v>278</v>
+      </c>
+      <c r="J115" s="35" t="s">
+        <v>328</v>
+      </c>
+      <c r="K115" s="54" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="A116" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="B116" s="35" t="s">
+        <v>281</v>
+      </c>
+      <c r="C116" s="35" t="s">
+        <v>330</v>
+      </c>
+      <c r="D116" s="54" t="s">
+        <v>331</v>
+      </c>
+      <c r="H116" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="I116" s="35" t="s">
+        <v>283</v>
+      </c>
+      <c r="J116" s="35" t="s">
+        <v>332</v>
+      </c>
+      <c r="K116" s="54" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="A117" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="B117" s="35" t="s">
+        <v>285</v>
+      </c>
+      <c r="C117" s="35" t="s">
+        <v>334</v>
+      </c>
+      <c r="D117" s="54" t="s">
+        <v>335</v>
+      </c>
+      <c r="H117" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="I117" s="35" t="s">
+        <v>287</v>
+      </c>
+      <c r="J117" s="35" t="s">
+        <v>336</v>
+      </c>
+      <c r="K117" s="54" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A118" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="B118" s="38"/>
+      <c r="C118" s="33"/>
+      <c r="D118" s="33"/>
+      <c r="H118" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="I118" s="38"/>
+      <c r="J118" s="33"/>
+      <c r="K118" s="33"/>
+    </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
 </worksheet>

</xml_diff>